<commit_message>
updates and cache logic update
</commit_message>
<xml_diff>
--- a/Project_Dashboard/cache.xlsx
+++ b/Project_Dashboard/cache.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>TOTAL AMOUNT</t>
+          <t xml:space="preserve">TOTAL AMOUNT </t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -486,7 +486,7 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>PACKING CHARGES</t>
+          <t xml:space="preserve">PACKING CHARGES </t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -496,12 +496,12 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>GRAND TOTAL</t>
+          <t xml:space="preserve"> GRAND TOTAL </t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>ADVANCE</t>
+          <t xml:space="preserve">ADVANCE </t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
@@ -5889,7 +5889,7 @@
         <v>0</v>
       </c>
       <c r="K94" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L94" t="n">
         <v>0</v>
@@ -5947,7 +5947,7 @@
         <v>0</v>
       </c>
       <c r="K95" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="L95" t="n">
         <v>0</v>
@@ -6005,7 +6005,7 @@
         <v>0</v>
       </c>
       <c r="K96" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="L96" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Data Types and column width Sorted
</commit_message>
<xml_diff>
--- a/Project_Dashboard/cache.xlsx
+++ b/Project_Dashboard/cache.xlsx
@@ -456,57 +456,57 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>TOTAL NO PCS.</t>
+          <t>total_pieces</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">TOTAL AMOUNT </t>
+          <t>total_amount</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>मूर्ति दुकान</t>
+          <t>murti_shop</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>गणेश लक्ष्मी दुकान</t>
+          <t>ganesh_lakshmi_shop</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>LOADING CHARGE</t>
+          <t>loading_charge</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>TRANSPORTATION</t>
+          <t>transportation</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">PACKING CHARGES </t>
+          <t>packing_charges</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>पहेले का बकाया</t>
+          <t>previous_balance</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> GRAND TOTAL </t>
+          <t>grand_total</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">ADVANCE </t>
+          <t>advance</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>PAYABLE</t>
+          <t>payable</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">

</xml_diff>